<commit_message>
se adiciona el formato de modelo conceptual
</commit_message>
<xml_diff>
--- a/sprint1/FORMATO SEGUIMIENTO-SPRINTS.xlsx
+++ b/sprint1/FORMATO SEGUIMIENTO-SPRINTS.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PLANEACIÓN-21082022" sheetId="2" r:id="rId1"/>
     <sheet name="DISTRIBUCIÓN-21082022" sheetId="3" r:id="rId2"/>
-    <sheet name="REUNION-01" sheetId="4" r:id="rId3"/>
+    <sheet name="REUNION-01-23082022" sheetId="4" r:id="rId3"/>
     <sheet name="REUNION-02" sheetId="6" r:id="rId4"/>
     <sheet name="REUNION-03" sheetId="5" r:id="rId5"/>
     <sheet name="REUNION-04" sheetId="7" r:id="rId6"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
   <si>
     <t>HACER</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>PEGAR EVIDENCIAS</t>
+  </si>
+  <si>
+    <t>TRELLO - GIRA - BETRIX</t>
+  </si>
+  <si>
+    <t>Requerimientos Usuario - RU - Daniel</t>
+  </si>
+  <si>
+    <t>Requerimientos No Funcionales - RNF - Erika</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +180,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,6 +274,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,6 +307,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>344650</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8382000" y="381000"/>
+          <a:ext cx="12536650" cy="5601482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G22"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,16 +638,16 @@
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="16" t="s">
         <v>2</v>
       </c>
     </row>
@@ -590,10 +684,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="6">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -604,10 +698,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="6">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -618,10 +712,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -632,10 +726,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="6">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -646,7 +740,6 @@
         <v>7</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -771,6 +864,11 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -783,7 +881,7 @@
   <dimension ref="B2:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,6 +921,7 @@
       <c r="C3" s="6">
         <v>10</v>
       </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
@@ -836,6 +935,7 @@
       <c r="C4" s="6">
         <v>5</v>
       </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
@@ -849,10 +949,10 @@
       <c r="C5" s="6">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
@@ -863,8 +963,9 @@
       <c r="C6" s="6">
         <v>65</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
+      <c r="D6" s="3"/>
+      <c r="E6" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -876,10 +977,10 @@
       <c r="C7" s="6">
         <v>10</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
@@ -1035,7 +1136,7 @@
   <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,6 +1414,9 @@
       <c r="G3" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
       <c r="I3" t="s">
         <v>20</v>
       </c>
@@ -1332,6 +1436,9 @@
       </c>
       <c r="G4" s="9" t="s">
         <v>12</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
       </c>
       <c r="I4" t="s">
         <v>20</v>
@@ -1459,6 +1566,10 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
+      <c r="H15">
+        <f>SUM(H3:H14)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
@@ -1799,5 +1910,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>